<commit_message>
Change Entity names for APIIT tests
</commit_message>
<xml_diff>
--- a/molgenis-data-rest/src/test/resources/RestControllerV1_API_TestEMX.xlsx
+++ b/molgenis-data-rest/src/test/resources/RestControllerV1_API_TestEMX.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="0" windowWidth="33860" windowHeight="18480"/>
+    <workbookView xWindow="1460" yWindow="0" windowWidth="33860" windowHeight="18480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
     <sheet name="entities" sheetId="3" r:id="rId2"/>
     <sheet name="attributes" sheetId="4" r:id="rId3"/>
-    <sheet name="V1_API_TypeTest" sheetId="1" r:id="rId4"/>
-    <sheet name="V1_API_TypeTestRef" sheetId="2" r:id="rId5"/>
+    <sheet name="V1_API_TypeTestAPIV1" sheetId="1" r:id="rId4"/>
+    <sheet name="V1_API_TypeTestRefAPIV1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -196,12 +196,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>TypeTest</t>
-  </si>
-  <si>
-    <t>TypeTestRef</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -448,9 +442,6 @@
     <t>abstract</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>{Chromosome: xstring, Position: xint}</t>
   </si>
   <si>
@@ -493,9 +484,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>Person</t>
-  </si>
-  <si>
     <t>AUTO</t>
   </si>
   <si>
@@ -817,22 +805,34 @@
     <t>MOLGENIS datatypes test package</t>
   </si>
   <si>
-    <t>V1_API_TypeTest</t>
-  </si>
-  <si>
-    <t>V1_API_Location</t>
-  </si>
-  <si>
-    <t>V1_API_Person</t>
-  </si>
-  <si>
-    <t>V1_API_TypeTestRef</t>
-  </si>
-  <si>
     <t>V1_API</t>
   </si>
   <si>
     <t>V1</t>
+  </si>
+  <si>
+    <t>TypeTestAPIV1</t>
+  </si>
+  <si>
+    <t>TypeTestRefAPIV1</t>
+  </si>
+  <si>
+    <t>LocationAPIV1</t>
+  </si>
+  <si>
+    <t>PersonAPIV1</t>
+  </si>
+  <si>
+    <t>V1_API_TypeTestRefAPIV1</t>
+  </si>
+  <si>
+    <t>V1_API_TypeTestAPIV1</t>
+  </si>
+  <si>
+    <t>V1_API_LocationAPIV1</t>
+  </si>
+  <si>
+    <t>V1_API_PersonAPIV1</t>
   </si>
 </sst>
 </file>
@@ -888,9 +888,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -959,7 +961,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="64">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1020,6 +1022,8 @@
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1322,7 +1326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -1340,28 +1344,27 @@
         <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1375,7 +1378,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1391,77 +1394,76 @@
         <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
         <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>263</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>264</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>265</v>
       </c>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1474,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1499,64 +1501,64 @@
         <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" t="s">
-        <v>83</v>
-      </c>
       <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" t="s">
+        <v>254</v>
+      </c>
+      <c r="O1" t="s">
         <v>90</v>
       </c>
-      <c r="M1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" t="s">
-        <v>258</v>
-      </c>
-      <c r="O1" t="s">
-        <v>92</v>
-      </c>
       <c r="P1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="R1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="T1" t="s">
         <v>56</v>
       </c>
       <c r="U1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1564,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1579,21 +1581,21 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="U2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1608,21 +1610,21 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="U3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1634,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1642,10 +1644,10 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -1660,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1668,10 +1670,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -1686,21 +1688,21 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="U6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1709,21 +1711,21 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="U7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1738,21 +1740,21 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="U8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1761,19 +1763,19 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="N9" t="b">
         <v>1</v>
       </c>
       <c r="Q9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="T9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="U9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1781,13 +1783,13 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1799,10 +1801,10 @@
         <v>2</v>
       </c>
       <c r="T10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="U10" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1810,13 +1812,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1828,21 +1830,21 @@
         <v>3</v>
       </c>
       <c r="T11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1851,27 +1853,27 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1880,10 +1882,10 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="T13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1891,10 +1893,10 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1909,10 +1911,10 @@
         <v>1</v>
       </c>
       <c r="T14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="U14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1920,10 +1922,10 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1935,10 +1937,10 @@
         <v>42095</v>
       </c>
       <c r="T15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="U15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1946,10 +1948,10 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1961,7 +1963,7 @@
         <v>6</v>
       </c>
       <c r="U16" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1969,10 +1971,10 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1987,10 +1989,10 @@
         <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="U17" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1998,10 +2000,10 @@
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -2016,10 +2018,10 @@
         <v>1</v>
       </c>
       <c r="T18" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="U18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -2027,10 +2029,10 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -2042,10 +2044,10 @@
         <v>15.666</v>
       </c>
       <c r="T19" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="U19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -2053,10 +2055,10 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -2065,16 +2067,16 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="N20" t="b">
         <v>1</v>
       </c>
       <c r="T20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="U20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -2082,10 +2084,10 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -2097,10 +2099,10 @@
         <v>7</v>
       </c>
       <c r="T21" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="U21" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -2108,10 +2110,10 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -2120,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H22" t="s">
         <v>8</v>
@@ -2129,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="T22" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -2137,10 +2139,10 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -2149,16 +2151,16 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
         <v>10</v>
       </c>
       <c r="T23" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="U23" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2166,10 +2168,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -2181,7 +2183,7 @@
         <v>11</v>
       </c>
       <c r="U24" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2189,10 +2191,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -2201,16 +2203,16 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="U25" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2218,10 +2220,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -2230,16 +2232,16 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="N26" t="b">
         <v>1</v>
       </c>
       <c r="T26" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="U26" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -2247,10 +2249,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -2259,13 +2261,13 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="T27" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="U27" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2273,10 +2275,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -2291,10 +2293,10 @@
         <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="U28" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2302,10 +2304,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -2317,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -2325,10 +2327,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -2343,10 +2345,10 @@
         <v>10</v>
       </c>
       <c r="T30" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="U30" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -2354,10 +2356,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -2372,10 +2374,10 @@
         <v>0</v>
       </c>
       <c r="T31" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="U31" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -2383,10 +2385,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -2398,10 +2400,10 @@
         <v>12342151234</v>
       </c>
       <c r="T32" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="U32" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -2409,10 +2411,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -2424,7 +2426,7 @@
         <v>12342151234</v>
       </c>
       <c r="U33" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -2432,10 +2434,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -2456,10 +2458,10 @@
         <v>1</v>
       </c>
       <c r="T34" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="U34" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -2467,10 +2469,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -2491,10 +2493,10 @@
         <v>1</v>
       </c>
       <c r="T35" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="U35" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -2502,13 +2504,13 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -2520,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="T36" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -2528,13 +2530,13 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -2548,10 +2550,10 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -2566,10 +2568,10 @@
         <v>1</v>
       </c>
       <c r="T38" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="U38" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -2577,10 +2579,10 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -2592,10 +2594,10 @@
         <v>39</v>
       </c>
       <c r="T39" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="U39" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -2603,7 +2605,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -2618,7 +2620,7 @@
         <v>40</v>
       </c>
       <c r="U40" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -2626,7 +2628,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -2641,10 +2643,10 @@
         <v>41</v>
       </c>
       <c r="T41" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U41" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -2652,13 +2654,13 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -2670,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="T42" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -2678,13 +2680,13 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -2693,18 +2695,18 @@
         <v>1</v>
       </c>
       <c r="T43" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:21">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -2719,21 +2721,21 @@
         <v>0</v>
       </c>
       <c r="T44" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="U44" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -2742,27 +2744,27 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="O45" t="b">
         <v>0</v>
       </c>
       <c r="T45" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="U45" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -2774,18 +2776,18 @@
         <v>1</v>
       </c>
       <c r="U46" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -2797,24 +2799,24 @@
         <v>1</v>
       </c>
       <c r="T47" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="U47" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B48" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -2826,18 +2828,18 @@
         <v>1</v>
       </c>
       <c r="T48" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:21">
       <c r="A49" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B49" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C49" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -2848,45 +2850,45 @@
     </row>
     <row r="50" spans="1:21">
       <c r="A50" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" t="s">
+        <v>267</v>
+      </c>
+      <c r="C50" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
         <v>139</v>
       </c>
-      <c r="B50" t="s">
-        <v>264</v>
-      </c>
-      <c r="C50" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="E50" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-      <c r="M50" t="b">
-        <v>1</v>
-      </c>
-      <c r="R50" t="s">
-        <v>142</v>
-      </c>
       <c r="T50" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="U50" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:21">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2901,21 +2903,21 @@
         <v>29</v>
       </c>
       <c r="T51" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="U51" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="b">
@@ -2936,18 +2938,18 @@
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="U52" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53" spans="1:21">
       <c r="A53" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="b">
@@ -2971,44 +2973,44 @@
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="U53" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:21">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E54" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
       </c>
       <c r="T54" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="U54" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:21">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -3017,21 +3019,21 @@
         <v>1</v>
       </c>
       <c r="T55" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="U55" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:21">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -3040,16 +3042,16 @@
         <v>1</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="S56" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="T56" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="U56" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3067,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3103,7 +3105,7 @@
   <sheetData>
     <row r="1" spans="1:45">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
@@ -3112,10 +3114,10 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
@@ -3124,10 +3126,10 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -3220,22 +3222,22 @@
         <v>43</v>
       </c>
       <c r="AN1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AO1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP1" t="s">
         <v>94</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>96</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>98</v>
-      </c>
       <c r="AR1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AS1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:45">
@@ -3252,7 +3254,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -3357,10 +3359,10 @@
         <v>2</v>
       </c>
       <c r="AN2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP2" t="s">
         <v>16</v>
@@ -3386,7 +3388,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -3491,10 +3493,10 @@
         <v>3</v>
       </c>
       <c r="AN3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP3" t="s">
         <v>17</v>
@@ -3517,7 +3519,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -3571,10 +3573,10 @@
         <v>4</v>
       </c>
       <c r="AN4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP4" t="s">
         <v>18</v>
@@ -3600,7 +3602,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -3705,13 +3707,13 @@
         <v>2</v>
       </c>
       <c r="AN5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AQ5">
         <v>4</v>
@@ -3734,7 +3736,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -3839,13 +3841,13 @@
         <v>3</v>
       </c>
       <c r="AN6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AQ6">
         <v>5</v>
@@ -3865,7 +3867,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -3919,13 +3921,13 @@
         <v>4</v>
       </c>
       <c r="AN7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AQ7">
         <v>6</v>
@@ -3945,7 +3947,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
@@ -4050,13 +4052,13 @@
         <v>2</v>
       </c>
       <c r="AN8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AQ8">
         <v>7</v>
@@ -4076,7 +4078,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
@@ -4181,13 +4183,13 @@
         <v>3</v>
       </c>
       <c r="AN9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AQ9">
         <v>8</v>
@@ -4204,7 +4206,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -4258,13 +4260,13 @@
         <v>4</v>
       </c>
       <c r="AN10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AQ10">
         <v>9</v>
@@ -4284,7 +4286,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -4389,13 +4391,13 @@
         <v>2</v>
       </c>
       <c r="AN11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AQ11">
         <v>10</v>
@@ -4415,7 +4417,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -4520,13 +4522,13 @@
         <v>3</v>
       </c>
       <c r="AN12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AQ12">
         <v>11</v>
@@ -4543,7 +4545,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
@@ -4597,13 +4599,13 @@
         <v>4</v>
       </c>
       <c r="AN13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AQ13">
         <v>12</v>
@@ -4623,7 +4625,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
         <v>2</v>
@@ -4728,13 +4730,13 @@
         <v>2</v>
       </c>
       <c r="AN14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AQ14">
         <v>13</v>
@@ -4754,7 +4756,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
@@ -4859,13 +4861,13 @@
         <v>3</v>
       </c>
       <c r="AN15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AQ15">
         <v>14</v>
@@ -4882,7 +4884,7 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
@@ -4936,13 +4938,13 @@
         <v>4</v>
       </c>
       <c r="AN16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AQ16">
         <v>15</v>
@@ -4959,7 +4961,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
@@ -5013,13 +5015,13 @@
         <v>4</v>
       </c>
       <c r="AN17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AQ17">
         <v>16</v>
@@ -5039,7 +5041,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -5144,13 +5146,13 @@
         <v>2</v>
       </c>
       <c r="AN18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AQ18">
         <v>17</v>
@@ -5170,7 +5172,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -5275,13 +5277,13 @@
         <v>3</v>
       </c>
       <c r="AN19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AQ19">
         <v>18</v>
@@ -5298,7 +5300,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -5352,13 +5354,13 @@
         <v>4</v>
       </c>
       <c r="AN20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AQ20">
         <v>19</v>
@@ -5378,7 +5380,7 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
@@ -5483,13 +5485,13 @@
         <v>2</v>
       </c>
       <c r="AN21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AO21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AQ21">
         <v>20</v>
@@ -5509,7 +5511,7 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F22" t="s">
         <v>3</v>
@@ -5614,10 +5616,10 @@
         <v>3</v>
       </c>
       <c r="AN22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AQ22">
         <v>21</v>
@@ -5634,7 +5636,7 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
@@ -5688,10 +5690,10 @@
         <v>4</v>
       </c>
       <c r="AN23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AQ23">
         <v>22</v>
@@ -5711,7 +5713,7 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -5816,10 +5818,10 @@
         <v>2</v>
       </c>
       <c r="AN24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AQ24">
         <v>23</v>
@@ -5839,7 +5841,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
         <v>3</v>
@@ -5944,10 +5946,10 @@
         <v>3</v>
       </c>
       <c r="AN25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AQ25">
         <v>24</v>
@@ -5964,7 +5966,7 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
@@ -6018,10 +6020,10 @@
         <v>4</v>
       </c>
       <c r="AN26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AQ26">
         <v>25</v>
@@ -6041,7 +6043,7 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F27" t="s">
         <v>2</v>
@@ -6146,10 +6148,10 @@
         <v>2</v>
       </c>
       <c r="AN27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AQ27">
         <v>26</v>
@@ -6169,7 +6171,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F28" t="s">
         <v>3</v>
@@ -6274,10 +6276,10 @@
         <v>3</v>
       </c>
       <c r="AN28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AQ28">
         <v>27</v>
@@ -6294,7 +6296,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -6348,10 +6350,10 @@
         <v>4</v>
       </c>
       <c r="AN29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AQ29">
         <v>28</v>
@@ -6371,7 +6373,7 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F30" t="s">
         <v>2</v>
@@ -6476,10 +6478,10 @@
         <v>2</v>
       </c>
       <c r="AN30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AQ30">
         <v>29</v>
@@ -6499,7 +6501,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -6604,10 +6606,10 @@
         <v>3</v>
       </c>
       <c r="AN31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AQ31">
         <v>30</v>
@@ -6624,7 +6626,7 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
@@ -6678,10 +6680,10 @@
         <v>4</v>
       </c>
       <c r="AN32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AQ32">
         <v>31</v>
@@ -6701,7 +6703,7 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F33" t="s">
         <v>2</v>
@@ -6806,10 +6808,10 @@
         <v>2</v>
       </c>
       <c r="AN33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AQ33">
         <v>32</v>
@@ -6829,7 +6831,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F34" t="s">
         <v>3</v>
@@ -6934,10 +6936,10 @@
         <v>3</v>
       </c>
       <c r="AN34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AQ34">
         <v>33</v>
@@ -6954,7 +6956,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
@@ -7008,10 +7010,10 @@
         <v>4</v>
       </c>
       <c r="AN35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AQ35">
         <v>34</v>
@@ -7028,7 +7030,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
@@ -7082,10 +7084,10 @@
         <v>4</v>
       </c>
       <c r="AN36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AQ36">
         <v>35</v>
@@ -7105,7 +7107,7 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F37" t="s">
         <v>2</v>
@@ -7210,10 +7212,10 @@
         <v>2</v>
       </c>
       <c r="AN37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AQ37">
         <v>36</v>
@@ -7233,7 +7235,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F38" t="s">
         <v>3</v>
@@ -7338,10 +7340,10 @@
         <v>3</v>
       </c>
       <c r="AN38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AQ38">
         <v>37</v>
@@ -7358,7 +7360,7 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F39" t="s">
         <v>4</v>
@@ -7412,10 +7414,10 @@
         <v>4</v>
       </c>
       <c r="AN39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AP39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AQ39">
         <v>38</v>
@@ -7572,7 +7574,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7580,7 +7582,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7588,7 +7590,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7596,7 +7598,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7604,7 +7606,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7612,7 +7614,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add separate entity for entity collection get tests
</commit_message>
<xml_diff>
--- a/molgenis-data-rest/src/test/resources/RestControllerV1_API_TestEMX.xlsx
+++ b/molgenis-data-rest/src/test/resources/RestControllerV1_API_TestEMX.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="0" windowWidth="33860" windowHeight="18480" activeTab="3"/>
+    <workbookView xWindow="1460" yWindow="0" windowWidth="33860" windowHeight="18480" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="attributes" sheetId="4" r:id="rId3"/>
     <sheet name="V1_API_TypeTestAPIV1" sheetId="1" r:id="rId4"/>
     <sheet name="V1_API_TypeTestRefAPIV1" sheetId="2" r:id="rId5"/>
+    <sheet name="V1_API_Items" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="272">
   <si>
     <t>text</t>
   </si>
@@ -833,6 +834,12 @@
   </si>
   <si>
     <t>V1_API_PersonAPIV1</t>
+  </si>
+  <si>
+    <t>V1_API_Items</t>
+  </si>
+  <si>
+    <t>Items</t>
   </si>
 </sst>
 </file>
@@ -888,9 +895,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -961,7 +972,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1024,6 +1035,10 @@
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1375,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1462,8 +1477,23 @@
         <v>258</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>271</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1474,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3054,6 +3084,61 @@
         <v>251</v>
       </c>
     </row>
+    <row r="57" spans="1:21">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>270</v>
+      </c>
+      <c r="C57" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" t="b">
+        <v>1</v>
+      </c>
+      <c r="T57" t="s">
+        <v>168</v>
+      </c>
+      <c r="U57" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" t="s">
+        <v>270</v>
+      </c>
+      <c r="C58" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="b">
+        <v>1</v>
+      </c>
+      <c r="L58" t="b">
+        <v>1</v>
+      </c>
+      <c r="T58" t="s">
+        <v>169</v>
+      </c>
+      <c r="U58" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3069,7 +3154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
@@ -7625,4 +7710,72 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>